<commit_message>
Update Lab 1 - Pumps documentation and fix typo in Lab 2 - Bolted Connections data file
</commit_message>
<xml_diff>
--- a/Lab 2 - Bolted Connections/data_and_analysis.xlsx
+++ b/Lab 2 - Bolted Connections/data_and_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\LaTeX\MEC-E-403\Lab 2 - Bolted Connections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EFBEA8F-FD9D-40F0-B68E-88B70F05263D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB516C40-46FD-49E2-BEA6-F8B91BF229D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="169">
   <si>
     <t>(V)</t>
   </si>
@@ -407,9 +407,6 @@
     <t>Bolt Stiffness and Washer Calibration (Nut Finger Tight)</t>
   </si>
   <si>
-    <t>Torque Test</t>
-  </si>
-  <si>
     <t>Bolt</t>
   </si>
   <si>
@@ -419,9 +416,6 @@
     <t>Repeatability at 50 lb-in torque (no external load)</t>
   </si>
   <si>
-    <t>Torque (in-lb)</t>
-  </si>
-  <si>
     <t>Trial 4</t>
   </si>
   <si>
@@ -461,9 +455,6 @@
     <t>in</t>
   </si>
   <si>
-    <t>Bolt Body Cross Sectional Area</t>
-  </si>
-  <si>
     <t>mm^2</t>
   </si>
   <si>
@@ -471,6 +462,111 @@
   </si>
   <si>
     <t>E</t>
+  </si>
+  <si>
+    <t>linest for bolt strain</t>
+  </si>
+  <si>
+    <t>linest for washer out</t>
+  </si>
+  <si>
+    <t>epsilon_{eq}</t>
+  </si>
+  <si>
+    <t>Gauge Resistance</t>
+  </si>
+  <si>
+    <t>Ω</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shunt Resistance </t>
+  </si>
+  <si>
+    <t>Number of Active Arms</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>correction factor</t>
+  </si>
+  <si>
+    <t>epsilon (coefficient for y = ax)</t>
+  </si>
+  <si>
+    <t>q2</t>
+  </si>
+  <si>
+    <t>Bolt Transducer, $V_b$</t>
+  </si>
+  <si>
+    <t>Washer Transducer, $V_w$</t>
+  </si>
+  <si>
+    <t>Bolt Strain, $\epsilon_b$</t>
+  </si>
+  <si>
+    <t>Preload, $F_i$</t>
+  </si>
+  <si>
+    <t>Torque, $T$ (Nm)</t>
+  </si>
+  <si>
+    <t>Torque, $T$ (in-lb)</t>
+  </si>
+  <si>
+    <t>linest for Preload vs Torque</t>
+  </si>
+  <si>
+    <t>Torque Coeff</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>bolt stiffness</t>
+  </si>
+  <si>
+    <t>k_0.910</t>
+  </si>
+  <si>
+    <t>k_1.471</t>
+  </si>
+  <si>
+    <t>Cross Sectional Area, $A_s$ (mm^2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bolt Body Cross Sectional Area of 0.910 </t>
+  </si>
+  <si>
+    <t>Bolt Body Cross Sectional Area of 1.471</t>
+  </si>
+  <si>
+    <t>Threaded Section Length</t>
+  </si>
+  <si>
+    <t>k_14.5</t>
+  </si>
+  <si>
+    <t>k_eff</t>
+  </si>
+  <si>
+    <t>Length of section, $L$</t>
+  </si>
+  <si>
+    <t>(in)</t>
+  </si>
+  <si>
+    <t>(mm)</t>
+  </si>
+  <si>
+    <t>1/k (m/MN)</t>
+  </si>
+  <si>
+    <t>Stiffness, $k$ (MN/m)</t>
+  </si>
+  <si>
+    <t>MN/m</t>
   </si>
 </sst>
 </file>
@@ -490,7 +586,7 @@
     <numFmt numFmtId="173" formatCode="#,##0.000000;\-#,##0.000000;\-"/>
     <numFmt numFmtId="174" formatCode="0.00000000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -526,13 +622,26 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -556,7 +665,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -660,36 +769,52 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1083,41 +1208,41 @@
       </c>
     </row>
     <row r="13" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="39" t="s">
+      <c r="D13" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="39"/>
-      <c r="G13" s="37" t="s">
+      <c r="E13" s="41"/>
+      <c r="G13" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
-      <c r="L13" s="39" t="s">
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
+      <c r="L13" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="M13" s="39"/>
+      <c r="M13" s="41"/>
       <c r="R13" s="3" t="s">
         <v>40</v>
       </c>
       <c r="S13" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="Z13" s="37" t="s">
+      <c r="Z13" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="AA13" s="37"/>
-      <c r="AB13" s="37" t="s">
+      <c r="AA13" s="42"/>
+      <c r="AB13" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="AC13" s="37"/>
-      <c r="AD13" s="37" t="s">
+      <c r="AC13" s="42"/>
+      <c r="AD13" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="AE13" s="37"/>
-      <c r="AF13" s="37" t="s">
+      <c r="AE13" s="42"/>
+      <c r="AF13" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="AG13" s="37"/>
+      <c r="AG13" s="42"/>
     </row>
     <row r="14" spans="1:39" s="16" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
@@ -1138,11 +1263,11 @@
       <c r="F14" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="38" t="s">
+      <c r="G14" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
       <c r="J14" s="18" t="s">
         <v>23</v>
       </c>
@@ -6158,8 +6283,8 @@
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
       <c r="H50" s="6"/>
-      <c r="K50" s="37"/>
-      <c r="L50" s="37"/>
+      <c r="K50" s="42"/>
+      <c r="L50" s="42"/>
       <c r="M50" s="8"/>
       <c r="N50" s="8"/>
     </row>
@@ -6184,8 +6309,8 @@
       <c r="F52" s="6"/>
       <c r="G52" s="6"/>
       <c r="H52" s="6"/>
-      <c r="K52" s="37"/>
-      <c r="L52" s="37"/>
+      <c r="K52" s="42"/>
+      <c r="L52" s="42"/>
       <c r="M52" s="8"/>
       <c r="N52" s="8"/>
     </row>
@@ -6232,37 +6357,37 @@
       <c r="N58" s="8"/>
     </row>
     <row r="59" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A59" s="39"/>
-      <c r="B59" s="37"/>
-      <c r="C59" s="39"/>
-      <c r="D59" s="39"/>
+      <c r="A59" s="41"/>
+      <c r="B59" s="42"/>
+      <c r="C59" s="41"/>
+      <c r="D59" s="41"/>
       <c r="E59" s="6"/>
-      <c r="F59" s="39"/>
-      <c r="G59" s="39"/>
-      <c r="H59" s="39"/>
-      <c r="K59" s="37"/>
-      <c r="L59" s="37"/>
+      <c r="F59" s="41"/>
+      <c r="G59" s="41"/>
+      <c r="H59" s="41"/>
+      <c r="K59" s="42"/>
+      <c r="L59" s="42"/>
       <c r="M59" s="8"/>
       <c r="N59" s="8"/>
     </row>
     <row r="60" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A60" s="39"/>
-      <c r="B60" s="37"/>
-      <c r="F60" s="39"/>
-      <c r="G60" s="39"/>
-      <c r="H60" s="39"/>
+      <c r="A60" s="41"/>
+      <c r="B60" s="42"/>
+      <c r="F60" s="41"/>
+      <c r="G60" s="41"/>
+      <c r="H60" s="41"/>
       <c r="M60" s="8"/>
       <c r="N60" s="8"/>
     </row>
     <row r="61" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A61" s="39"/>
-      <c r="C61" s="37"/>
-      <c r="D61" s="37"/>
-      <c r="F61" s="37"/>
-      <c r="G61" s="37"/>
-      <c r="H61" s="37"/>
-      <c r="K61" s="37"/>
-      <c r="L61" s="37"/>
+      <c r="A61" s="41"/>
+      <c r="C61" s="42"/>
+      <c r="D61" s="42"/>
+      <c r="F61" s="42"/>
+      <c r="G61" s="42"/>
+      <c r="H61" s="42"/>
+      <c r="K61" s="42"/>
+      <c r="L61" s="42"/>
       <c r="M61" s="8"/>
       <c r="N61" s="8"/>
     </row>
@@ -6284,14 +6409,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="F59:H60"/>
-    <mergeCell ref="K59:L59"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="F61:H61"/>
-    <mergeCell ref="K61:L61"/>
     <mergeCell ref="AF13:AG13"/>
     <mergeCell ref="G14:I14"/>
     <mergeCell ref="K50:L50"/>
@@ -6302,6 +6419,14 @@
     <mergeCell ref="Z13:AA13"/>
     <mergeCell ref="AB13:AC13"/>
     <mergeCell ref="AD13:AE13"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="F59:H60"/>
+    <mergeCell ref="K59:L59"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="F61:H61"/>
+    <mergeCell ref="K61:L61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6494,41 +6619,41 @@
       </c>
     </row>
     <row r="13" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="D13" s="39" t="s">
+      <c r="D13" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="39"/>
-      <c r="G13" s="37" t="s">
+      <c r="E13" s="41"/>
+      <c r="G13" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
-      <c r="L13" s="39" t="s">
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
+      <c r="L13" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="M13" s="39"/>
+      <c r="M13" s="41"/>
       <c r="R13" s="3" t="s">
         <v>40</v>
       </c>
       <c r="S13" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="Z13" s="37" t="s">
+      <c r="Z13" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="AA13" s="37"/>
-      <c r="AB13" s="37" t="s">
+      <c r="AA13" s="42"/>
+      <c r="AB13" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="AC13" s="37"/>
-      <c r="AD13" s="37" t="s">
+      <c r="AC13" s="42"/>
+      <c r="AD13" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="AE13" s="37"/>
-      <c r="AF13" s="37" t="s">
+      <c r="AE13" s="42"/>
+      <c r="AF13" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="AG13" s="37"/>
+      <c r="AG13" s="42"/>
       <c r="AO13" s="3" t="s">
         <v>83</v>
       </c>
@@ -6552,11 +6677,11 @@
       <c r="F14" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="38" t="s">
+      <c r="G14" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
       <c r="J14" s="18" t="s">
         <v>23</v>
       </c>
@@ -11784,16 +11909,16 @@
       </c>
     </row>
     <row r="54" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="C54" s="37" t="s">
+      <c r="C54" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="D54" s="37"/>
-      <c r="E54" s="37"/>
-      <c r="F54" s="37" t="s">
+      <c r="D54" s="42"/>
+      <c r="E54" s="42"/>
+      <c r="F54" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="G54" s="37"/>
-      <c r="H54" s="37"/>
+      <c r="G54" s="42"/>
+      <c r="H54" s="42"/>
     </row>
     <row r="55" spans="1:39" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C55" s="17" t="s">
@@ -13980,785 +14105,1179 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{712A8C4D-2617-403C-8503-1436772C4FFD}">
-  <dimension ref="A1:H67"/>
+  <dimension ref="A1:K119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.140625" style="42" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="42" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="9.140625" style="42"/>
-    <col min="6" max="6" width="12.7109375" style="42" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="42"/>
+    <col min="1" max="1" width="50.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="40" t="s">
+    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="41">
+      <c r="B1" s="38">
         <v>400</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="40" t="s">
+      <c r="E1" s="39" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="B2" s="41">
+      <c r="B2" s="38">
         <v>0.34300000000000003</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="40" t="s">
+      <c r="E2" s="53">
+        <f>75-(0.91+1.471)*25.4</f>
+        <v>14.522599999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="37" t="s">
         <v>108</v>
       </c>
-      <c r="B3" s="41">
+      <c r="B3" s="38">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="40" t="s">
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="B4" s="41">
+      <c r="B4" s="38">
         <v>0.375</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="40" t="s">
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="B5" s="41">
+      <c r="B5" s="38">
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="40" t="s">
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="37" t="s">
+        <v>127</v>
+      </c>
+      <c r="B6" s="38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="B7" s="38">
+        <v>0.371</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" s="37" t="s">
         <v>129</v>
       </c>
-      <c r="B6" s="41">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="40" t="s">
+      <c r="B8" s="38">
+        <v>0.155</v>
+      </c>
+      <c r="C8" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="B7" s="41">
-        <v>0.371</v>
-      </c>
-      <c r="C7" s="43" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="40" t="s">
-        <v>131</v>
-      </c>
-      <c r="B8" s="41">
-        <v>0.155</v>
-      </c>
-      <c r="C8" s="43" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="40" t="s">
-        <v>133</v>
-      </c>
-      <c r="B9" s="41">
+    </row>
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A9" s="37" t="s">
+        <v>158</v>
+      </c>
+      <c r="B9" s="38">
         <f>PI()/4*(B7^2-B8^2)*(25.4)^2</f>
         <v>57.570076945141288</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="39" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A10" s="37" t="s">
+        <v>159</v>
+      </c>
+      <c r="B10" s="38">
+        <f>PI()/4*B7^2*25.4^2</f>
+        <v>69.743724130458673</v>
+      </c>
+      <c r="C10" s="39"/>
+    </row>
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A11" s="37" t="s">
+        <v>159</v>
+      </c>
+      <c r="B11" s="38">
+        <f>PI()/4*B4^2*25.4^2</f>
+        <v>71.255739248085618</v>
+      </c>
+      <c r="C11" s="39"/>
+    </row>
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12" s="38">
+        <v>120</v>
+      </c>
+      <c r="C12" s="38" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A13" s="37" t="s">
+        <v>139</v>
+      </c>
+      <c r="B13" s="38">
+        <v>175000</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A14" s="37" t="s">
+        <v>140</v>
+      </c>
+      <c r="B14" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A17" s="49" t="s">
+        <v>114</v>
+      </c>
+      <c r="B17" s="45"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="44" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="43" t="s">
+      <c r="H17" s="45"/>
+    </row>
+    <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A18" s="49" t="s">
+        <v>111</v>
+      </c>
+      <c r="B18" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="C18" s="44" t="s">
+        <v>113</v>
+      </c>
+      <c r="D18" s="44" t="s">
+        <v>126</v>
+      </c>
+      <c r="F18" s="45" t="s">
+        <v>132</v>
+      </c>
+      <c r="G18" s="45" cm="1">
+        <f t="array" ref="G18:H22">LINEST(D19:D27,A19:A27, FALSE, TRUE)</f>
+        <v>8.4713375796178328E-5</v>
+      </c>
+      <c r="H18" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A19" s="45">
+        <v>0</v>
+      </c>
+      <c r="B19" s="46">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="C19" s="45">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+      <c r="D19" s="47">
+        <f>4*B19/($B$6*$B$3*$B$1)</f>
+        <v>6.0000000000000002E-6</v>
+      </c>
+      <c r="G19">
+        <v>8.2056660109804756E-7</v>
+      </c>
+      <c r="H19" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A20" s="45">
+        <v>1</v>
+      </c>
+      <c r="B20" s="46">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="C20" s="45">
+        <v>-0.21199999999999999</v>
+      </c>
+      <c r="D20" s="47">
+        <f t="shared" ref="D20:D27" si="0">4*B20/($B$6*$B$3*$B$1)</f>
+        <v>8.5000000000000006E-5</v>
+      </c>
+      <c r="G20">
+        <v>0.99924995413810469</v>
+      </c>
+      <c r="H20">
+        <v>1.1495256568118845E-5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A21" s="45">
+        <v>2</v>
+      </c>
+      <c r="B21" s="46">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="C21" s="45">
+        <v>-0.441</v>
+      </c>
+      <c r="D21" s="47">
+        <f t="shared" si="0"/>
+        <v>1.6800000000000002E-4</v>
+      </c>
+      <c r="G21">
+        <v>10658.014448481304</v>
+      </c>
+      <c r="H21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A22" s="45">
+        <v>3</v>
+      </c>
+      <c r="B22" s="46">
+        <v>0.253</v>
+      </c>
+      <c r="C22" s="45">
+        <v>-0.66700000000000004</v>
+      </c>
+      <c r="D22" s="47">
+        <f t="shared" si="0"/>
+        <v>2.5300000000000002E-4</v>
+      </c>
+      <c r="G22">
+        <v>1.4083598726114649E-6</v>
+      </c>
+      <c r="H22">
+        <v>1.0571273885350356E-9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A23" s="45">
+        <v>4</v>
+      </c>
+      <c r="B23" s="46">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="C23" s="45">
+        <v>-0.88800000000000001</v>
+      </c>
+      <c r="D23" s="47">
+        <f t="shared" si="0"/>
+        <v>3.3500000000000001E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A24" s="45">
+        <v>5</v>
+      </c>
+      <c r="B24" s="46">
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="C24" s="45">
+        <v>-1.08</v>
+      </c>
+      <c r="D24" s="47">
+        <f t="shared" si="0"/>
+        <v>4.17E-4</v>
+      </c>
+      <c r="F24" s="50" t="s">
+        <v>133</v>
+      </c>
+      <c r="G24" s="51">
+        <f>1/(G18*B9)</f>
+        <v>205.04595276890194</v>
+      </c>
+      <c r="H24" s="52" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A25" s="45">
+        <v>6</v>
+      </c>
+      <c r="B25" s="46">
+        <v>0.498</v>
+      </c>
+      <c r="C25" s="45">
+        <v>-1.27</v>
+      </c>
+      <c r="D25" s="47">
+        <f t="shared" si="0"/>
+        <v>4.9799999999999996E-4</v>
+      </c>
+      <c r="F25" s="44"/>
+      <c r="G25" s="44" t="s">
+        <v>135</v>
+      </c>
+      <c r="H25" s="45"/>
+    </row>
+    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A26" s="45">
+        <v>7</v>
+      </c>
+      <c r="B26" s="46">
+        <v>0.58099999999999996</v>
+      </c>
+      <c r="C26" s="45">
+        <v>-1.46</v>
+      </c>
+      <c r="D26" s="47">
+        <f t="shared" si="0"/>
+        <v>5.8099999999999992E-4</v>
+      </c>
+      <c r="F26" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="G26" s="45" cm="1">
+        <f t="array" ref="G26:H26">LINEST(C19:C27,A19:A27, FALSE)</f>
+        <v>-0.21141146496815286</v>
+      </c>
+      <c r="H26" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A27" s="45">
+        <v>7.5</v>
+      </c>
+      <c r="B27" s="46">
+        <v>0.66200000000000003</v>
+      </c>
+      <c r="C27" s="45">
+        <v>-1.5469999999999999</v>
+      </c>
+      <c r="D27" s="47">
+        <f t="shared" si="0"/>
+        <v>6.6200000000000005E-4</v>
+      </c>
+      <c r="F27" s="48" t="s">
+        <v>143</v>
+      </c>
+      <c r="G27" s="45">
+        <f>4*G26/(B6*B3*B1)</f>
+        <v>-2.1141146496815285E-4</v>
+      </c>
+      <c r="H27" s="45"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F29" s="50" t="s">
+        <v>136</v>
+      </c>
+      <c r="G29" s="51">
+        <f>B12/(B14*B6*(B13+B12))</f>
+        <v>3.4262220191868436E-4</v>
+      </c>
+      <c r="H29" s="50" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F30" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="G30" s="45">
+        <f>G18/G27</f>
+        <v>-0.40070379252581972</v>
+      </c>
+      <c r="H30" s="45"/>
+    </row>
+    <row r="32" spans="1:9" s="56" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A32" s="55" t="s">
+        <v>111</v>
+      </c>
+      <c r="B32" s="55" t="s">
+        <v>150</v>
+      </c>
+      <c r="C32" s="55" t="s">
+        <v>149</v>
+      </c>
+      <c r="D32" s="55" t="s">
+        <v>145</v>
+      </c>
+      <c r="E32" s="55" t="s">
+        <v>146</v>
+      </c>
+      <c r="F32" s="55" t="s">
+        <v>147</v>
+      </c>
+      <c r="G32" s="55" t="s">
+        <v>148</v>
+      </c>
+      <c r="H32" s="57"/>
+      <c r="I32" s="55" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>0</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <f>B33*0.11298482933333</f>
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>-2E-3</v>
+      </c>
+      <c r="E33">
+        <v>-1E-3</v>
+      </c>
+      <c r="F33" s="40">
+        <f>4*D33/($B$6*$B$3*$B$1)</f>
+        <v>-1.9999999999999999E-6</v>
+      </c>
+      <c r="G33" s="40">
+        <f>$G$24*F33*$B$9</f>
+        <v>-2.3609022556390982E-2</v>
+      </c>
+      <c r="I33" cm="1">
+        <f t="array" ref="I33:J37">LINEST(G33:G38,C33:C38, FALSE, TRUE)</f>
+        <v>0.63576255935467008</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>0</v>
+      </c>
+      <c r="B34">
+        <v>25</v>
+      </c>
+      <c r="C34">
+        <f t="shared" ref="C34:C38" si="1">B34*0.11298482933333</f>
+        <v>2.82462073333325</v>
+      </c>
+      <c r="D34">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E34">
+        <v>-0.311</v>
+      </c>
+      <c r="F34" s="40">
+        <f t="shared" ref="F34:F38" si="2">4*D34/($B$6*$B$3*$B$1)</f>
+        <v>1.4000000000000001E-4</v>
+      </c>
+      <c r="G34" s="54">
+        <f t="shared" ref="G34:G38" si="3">$G$24*F34*$B$9</f>
+        <v>1.6526315789473691</v>
+      </c>
+      <c r="I34">
+        <v>6.6107414151537879E-3</v>
+      </c>
+      <c r="J34" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>0</v>
+      </c>
+      <c r="B35">
+        <v>50</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="1"/>
+        <v>5.6492414666665001</v>
+      </c>
+      <c r="D35">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="E35">
+        <v>-0.61499999999999999</v>
+      </c>
+      <c r="F35" s="40">
+        <f t="shared" si="2"/>
+        <v>2.9399999999999999E-4</v>
+      </c>
+      <c r="G35" s="54">
+        <f t="shared" si="3"/>
+        <v>3.4705263157894746</v>
+      </c>
+      <c r="I35">
+        <v>0.99945968661223894</v>
+      </c>
+      <c r="J35">
+        <v>0.138481467466676</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>0</v>
+      </c>
+      <c r="B36">
+        <v>75</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="1"/>
+        <v>8.4738621999997505</v>
+      </c>
+      <c r="D36">
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="E36">
+        <v>-0.90700000000000003</v>
+      </c>
+      <c r="F36" s="40">
+        <f t="shared" si="2"/>
+        <v>4.4700000000000002E-4</v>
+      </c>
+      <c r="G36" s="54">
+        <f t="shared" si="3"/>
+        <v>5.276616541353385</v>
+      </c>
+      <c r="I36">
+        <v>9248.8887861332005</v>
+      </c>
+      <c r="J36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>0</v>
+      </c>
+      <c r="B37">
+        <v>100</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="1"/>
+        <v>11.298482933333</v>
+      </c>
+      <c r="D37">
+        <v>0.60199999999999998</v>
+      </c>
+      <c r="E37">
+        <v>-1.2030000000000001</v>
+      </c>
+      <c r="F37" s="40">
+        <f t="shared" si="2"/>
+        <v>6.02E-4</v>
+      </c>
+      <c r="G37" s="54">
+        <f t="shared" si="3"/>
+        <v>7.106315789473685</v>
+      </c>
+      <c r="H37" s="40"/>
+      <c r="I37">
+        <v>177.36702081529876</v>
+      </c>
+      <c r="J37">
+        <v>9.5885584158620224E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>0</v>
+      </c>
+      <c r="B38">
+        <v>125</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="1"/>
+        <v>14.12310366666625</v>
+      </c>
+      <c r="D38">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="E38">
+        <v>-1.5189999999999999</v>
+      </c>
+      <c r="F38" s="40">
+        <f t="shared" si="2"/>
+        <v>7.7800000000000005E-4</v>
+      </c>
+      <c r="G38" s="54">
+        <f t="shared" si="3"/>
+        <v>9.1839097744360938</v>
+      </c>
+      <c r="H38" s="54"/>
+      <c r="I38" s="58" t="s">
+        <v>152</v>
+      </c>
+      <c r="J38" s="59">
+        <f>1/(I33*B7*25.4)</f>
+        <v>0.16691579121627786</v>
+      </c>
+      <c r="K38" s="58" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="60" t="s">
+        <v>163</v>
+      </c>
+      <c r="C40" s="60"/>
+    </row>
+    <row r="41" spans="1:11" s="56" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A41" s="55" t="s">
+        <v>154</v>
+      </c>
+      <c r="B41" s="55" t="s">
+        <v>164</v>
+      </c>
+      <c r="C41" s="55" t="s">
+        <v>165</v>
+      </c>
+      <c r="D41" s="55" t="s">
+        <v>157</v>
+      </c>
+      <c r="E41" s="55" t="s">
+        <v>167</v>
+      </c>
+      <c r="F41" s="55" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" s="56" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="39" t="s">
+        <v>155</v>
+      </c>
+      <c r="B42" s="39">
+        <v>0.91</v>
+      </c>
+      <c r="C42" s="56">
+        <f>25.4*B42</f>
+        <v>23.114000000000001</v>
+      </c>
+      <c r="D42" s="56">
+        <f>B9</f>
+        <v>57.570076945141288</v>
+      </c>
+      <c r="E42" s="56">
+        <f>D42*$G$24/C42</f>
+        <v>510.70828407871807</v>
+      </c>
+      <c r="F42" s="56">
+        <f>1/E42</f>
+        <v>1.9580649681528663E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43" s="39" t="s">
+        <v>156</v>
+      </c>
+      <c r="B43" s="39">
+        <v>1.4710000000000001</v>
+      </c>
+      <c r="C43" s="56">
+        <f>25.4*B43</f>
+        <v>37.363399999999999</v>
+      </c>
+      <c r="D43" s="56">
+        <f t="shared" ref="D43:D44" si="4">B10</f>
+        <v>69.743724130458673</v>
+      </c>
+      <c r="E43" s="56">
+        <f t="shared" ref="E43" si="5">D43*$G$24/C43</f>
+        <v>382.74537017459215</v>
+      </c>
+      <c r="F43" s="56">
+        <f t="shared" ref="F43:F44" si="6">1/E43</f>
+        <v>2.6127030603762562E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A44" s="39" t="s">
+        <v>161</v>
+      </c>
+      <c r="B44" s="53">
+        <f>E2/25.4</f>
+        <v>0.57175590551181099</v>
+      </c>
+      <c r="C44" s="56">
+        <f>25.4*B44</f>
+        <v>14.522599999999999</v>
+      </c>
+      <c r="D44" s="56">
+        <f t="shared" si="4"/>
+        <v>71.255739248085618</v>
+      </c>
+      <c r="E44" s="56">
+        <f>D44*$G$24/C44</f>
+        <v>1006.0664718697863</v>
+      </c>
+      <c r="F44" s="56">
+        <f t="shared" si="6"/>
+        <v>9.9397010829859822E-4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A46" s="55" t="s">
+        <v>162</v>
+      </c>
+      <c r="B46">
+        <f>(SUM(F42:F44))^(-1)</f>
+        <v>179.70297530838855</v>
+      </c>
+      <c r="C46" s="39" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="B70" s="39"/>
+    </row>
+    <row r="71" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A71" s="39"/>
+      <c r="B71" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="C71" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="D71" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="E71" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="F71" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="G71" s="38"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="B72">
+        <v>0.372</v>
+      </c>
+      <c r="C72">
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="D72">
+        <v>0.35399999999999998</v>
+      </c>
+      <c r="E72">
+        <v>0.312</v>
+      </c>
+      <c r="F72">
+        <v>0.32700000000000001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="B73">
+        <v>-0.70099999999999996</v>
+      </c>
+      <c r="C73">
+        <v>-0.68400000000000005</v>
+      </c>
+      <c r="D73">
+        <v>-0.71799999999999997</v>
+      </c>
+      <c r="E73">
+        <v>-0.65400000000000003</v>
+      </c>
+      <c r="F73">
+        <v>-0.67900000000000005</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E75" s="45"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E76" s="45"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E77" s="45"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E78" s="45"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E79" s="45"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E80" s="45"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E81" s="45"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E82" s="45"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E83" s="45"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E84" s="45"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E85" s="45"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87" s="39" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88" s="39" t="s">
+        <v>121</v>
+      </c>
+      <c r="B88" s="39" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89" s="39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A90" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="C11" s="47" t="s">
-        <v>119</v>
-      </c>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="47"/>
-      <c r="H11" s="47"/>
-    </row>
-    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="43"/>
-      <c r="C12" s="46">
-        <v>0</v>
-      </c>
-      <c r="D12" s="45">
-        <v>25</v>
-      </c>
-      <c r="E12" s="42">
-        <v>50</v>
-      </c>
-      <c r="F12" s="45">
-        <v>75</v>
-      </c>
-      <c r="G12" s="45">
-        <v>100</v>
-      </c>
-      <c r="H12" s="45">
+      <c r="B90" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="C90" s="39" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A91" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="B91" s="38">
+        <v>0.38600000000000001</v>
+      </c>
+      <c r="C91">
+        <v>-0.73099999999999998</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A92" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="B92" s="38">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="C92">
+        <v>-0.72</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A93" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="B93" s="38">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="C93">
+        <v>-0.71499999999999997</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>0</v>
+      </c>
+      <c r="B94" s="38">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="C94">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>1</v>
+      </c>
+      <c r="B95" s="38">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="C95">
+        <v>-0.751</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>2</v>
+      </c>
+      <c r="B96" s="38">
+        <v>0.4</v>
+      </c>
+      <c r="C96">
+        <v>-0.78300000000000003</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>3</v>
+      </c>
+      <c r="B97" s="38">
+        <v>0.41099999999999998</v>
+      </c>
+      <c r="C97">
+        <v>-0.81799999999999995</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>4</v>
+      </c>
+      <c r="B98" s="38">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="C98">
+        <v>-0.85499999999999998</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>5</v>
+      </c>
+      <c r="B99" s="38">
+        <v>0.436</v>
+      </c>
+      <c r="C99">
+        <v>-0.90100000000000002</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>6</v>
+      </c>
+      <c r="B100" s="38">
+        <v>0.498</v>
+      </c>
+      <c r="C100">
+        <v>-1.0680000000000001</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>7</v>
+      </c>
+      <c r="B101" s="38">
+        <v>0.57799999999999996</v>
+      </c>
+      <c r="C101">
+        <v>-1.226</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>7.5</v>
+      </c>
+      <c r="B102" s="38">
+        <v>0.61899999999999999</v>
+      </c>
+      <c r="C102">
+        <v>-1.3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" s="39" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C13" s="42">
-        <f>C12*0.112984829</f>
-        <v>0</v>
-      </c>
-      <c r="D13" s="42">
-        <f t="shared" ref="D13:H13" si="0">D12*0.112984829</f>
-        <v>2.8246207249999999</v>
-      </c>
-      <c r="E13" s="42">
-        <f t="shared" si="0"/>
-        <v>5.6492414499999999</v>
-      </c>
-      <c r="F13" s="42">
-        <f t="shared" si="0"/>
-        <v>8.4738621749999989</v>
-      </c>
-      <c r="G13" s="42">
-        <f t="shared" si="0"/>
-        <v>11.2984829</v>
-      </c>
-      <c r="H13" s="42">
-        <f t="shared" si="0"/>
-        <v>14.123103624999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="43" t="s">
-        <v>116</v>
-      </c>
-      <c r="B14" s="42">
-        <v>0</v>
-      </c>
-      <c r="C14" s="42">
-        <v>-2E-3</v>
-      </c>
-      <c r="D14" s="42">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="E14" s="42">
-        <v>0.29399999999999998</v>
-      </c>
-      <c r="F14" s="45">
-        <v>0.44700000000000001</v>
-      </c>
-      <c r="G14" s="45">
-        <v>0.60199999999999998</v>
-      </c>
-      <c r="H14" s="45">
-        <v>0.77800000000000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="43" t="s">
-        <v>117</v>
-      </c>
-      <c r="B15" s="42">
-        <v>0</v>
-      </c>
-      <c r="C15" s="42">
-        <v>-1E-3</v>
-      </c>
-      <c r="D15" s="42">
-        <v>-0.311</v>
-      </c>
-      <c r="E15" s="42">
-        <v>-0.61499999999999999</v>
-      </c>
-      <c r="F15" s="45">
-        <v>-0.90700000000000003</v>
-      </c>
-      <c r="G15" s="45">
-        <v>-1.2030000000000001</v>
-      </c>
-      <c r="H15" s="45">
-        <v>-1.5189999999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="43" t="s">
-        <v>118</v>
-      </c>
-      <c r="B18" s="43"/>
-    </row>
-    <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="43"/>
-      <c r="B19" s="46" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="46" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" s="46" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" s="46" t="s">
-        <v>120</v>
-      </c>
-      <c r="F19" s="46" t="s">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" s="39" t="s">
         <v>121</v>
       </c>
-      <c r="G19" s="46"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="43" t="s">
-        <v>116</v>
-      </c>
-      <c r="B20" s="42">
-        <v>0.372</v>
-      </c>
-      <c r="C20" s="42">
+      <c r="B105" s="39" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" s="39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A107" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="B107" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="C107" s="39" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A108" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="B108" s="38">
+        <v>0.32700000000000001</v>
+      </c>
+      <c r="C108">
+        <v>-0.54</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A109" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="B109" s="38">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="C109">
+        <v>-0.53400000000000003</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A110" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="B110" s="38">
         <v>0.32100000000000001</v>
       </c>
-      <c r="D20" s="42">
-        <v>0.35399999999999998</v>
-      </c>
-      <c r="E20" s="42">
-        <v>0.312</v>
-      </c>
-      <c r="F20" s="42">
-        <v>0.32700000000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="43" t="s">
-        <v>117</v>
-      </c>
-      <c r="B21" s="42">
-        <v>-0.70099999999999996</v>
-      </c>
-      <c r="C21" s="42">
-        <v>-0.68400000000000005</v>
-      </c>
-      <c r="D21" s="42">
-        <v>-0.71799999999999997</v>
-      </c>
-      <c r="E21" s="45">
-        <v>-0.65400000000000003</v>
-      </c>
-      <c r="F21" s="45">
-        <v>-0.67900000000000005</v>
-      </c>
-      <c r="G21" s="45"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E22" s="45"/>
-      <c r="F22" s="45"/>
-      <c r="G22" s="45"/>
-    </row>
-    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A23" s="44" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A24" s="44" t="s">
-        <v>111</v>
-      </c>
-      <c r="B24" s="43" t="s">
-        <v>112</v>
-      </c>
-      <c r="C24" s="43" t="s">
-        <v>113</v>
-      </c>
-      <c r="D24" s="43" t="s">
-        <v>128</v>
-      </c>
-      <c r="F24" s="50" t="s">
-        <v>135</v>
-      </c>
-      <c r="G24" s="42" cm="1">
-        <f t="array" ref="G24:H24">LINEST(D25:D33,A25:A33)</f>
-        <v>8.4876482213438754E-5</v>
-      </c>
-      <c r="H24" s="42">
-        <v>-9.0167984189733338E-7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A25" s="42">
-        <v>0</v>
-      </c>
-      <c r="B25" s="46">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="C25" s="42">
-        <v>-3.0000000000000001E-3</v>
-      </c>
-      <c r="D25" s="49">
-        <f>4*B25/($B$6*$B$3*$B$1)</f>
-        <v>6.0000000000000002E-6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26" s="42">
+      <c r="C110">
+        <v>-0.53</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>0</v>
+      </c>
+      <c r="B111" s="38">
+        <v>0.315</v>
+      </c>
+      <c r="C111">
+        <v>-0.52800000000000002</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A112">
         <v>1</v>
       </c>
-      <c r="B26" s="46">
-        <v>8.5000000000000006E-2</v>
-      </c>
-      <c r="C26" s="42">
-        <v>-0.21199999999999999</v>
-      </c>
-      <c r="D26" s="49">
-        <f t="shared" ref="D26:D33" si="1">4*B26/($B$6*$B$3*$B$1)</f>
-        <v>8.5000000000000006E-5</v>
-      </c>
-      <c r="F26" s="43" t="s">
-        <v>136</v>
-      </c>
-      <c r="G26" s="42">
-        <f>1/(G24*B9)</f>
-        <v>204.6519176974933</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A27" s="42">
+      <c r="B112" s="38">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="C112">
+        <v>-0.59299999999999997</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A113">
         <v>2</v>
       </c>
-      <c r="B27" s="46">
-        <v>0.16800000000000001</v>
-      </c>
-      <c r="C27" s="42">
-        <v>-0.441</v>
-      </c>
-      <c r="D27" s="49">
-        <f t="shared" si="1"/>
-        <v>1.6800000000000002E-4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A28" s="45">
+      <c r="B113" s="38">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="C113">
+        <v>-0.67400000000000004</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A114">
         <v>3</v>
       </c>
-      <c r="B28" s="46">
-        <v>0.253</v>
-      </c>
-      <c r="C28" s="45">
-        <v>-0.66700000000000004</v>
-      </c>
-      <c r="D28" s="49">
-        <f t="shared" si="1"/>
-        <v>2.5300000000000002E-4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A29" s="45">
+      <c r="B114" s="38">
+        <v>0.38900000000000001</v>
+      </c>
+      <c r="C114">
+        <v>-0.76600000000000001</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A115">
         <v>4</v>
       </c>
-      <c r="B29" s="46">
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="C29" s="45">
-        <v>-0.88800000000000001</v>
-      </c>
-      <c r="D29" s="49">
-        <f t="shared" si="1"/>
-        <v>3.3500000000000001E-4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A30" s="45">
+      <c r="B115" s="38">
+        <v>0.42599999999999999</v>
+      </c>
+      <c r="C115">
+        <v>-0.85599999999999998</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A116">
         <v>5</v>
       </c>
-      <c r="B30" s="46">
-        <v>0.41699999999999998</v>
-      </c>
-      <c r="C30" s="45">
-        <v>-1.08</v>
-      </c>
-      <c r="D30" s="49">
-        <f t="shared" si="1"/>
-        <v>4.17E-4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A31" s="45">
+      <c r="B116" s="38">
+        <v>0.46899999999999997</v>
+      </c>
+      <c r="C116">
+        <v>-0.94099999999999995</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A117">
         <v>6</v>
       </c>
-      <c r="B31" s="46">
-        <v>0.498</v>
-      </c>
-      <c r="C31" s="45">
-        <v>-1.27</v>
-      </c>
-      <c r="D31" s="49">
-        <f t="shared" si="1"/>
-        <v>4.9799999999999996E-4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A32" s="45">
+      <c r="B117" s="38">
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="C117">
+        <v>-1.036</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A118">
         <v>7</v>
       </c>
-      <c r="B32" s="46">
-        <v>0.58099999999999996</v>
-      </c>
-      <c r="C32" s="45">
-        <v>-1.46</v>
-      </c>
-      <c r="D32" s="49">
-        <f t="shared" si="1"/>
-        <v>5.8099999999999992E-4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A33" s="45">
+      <c r="B118" s="38">
+        <v>0.58899999999999997</v>
+      </c>
+      <c r="C118">
+        <v>-1.1479999999999999</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A119">
         <v>7.5</v>
       </c>
-      <c r="B33" s="46">
-        <v>0.66200000000000003</v>
-      </c>
-      <c r="C33" s="45">
-        <v>-1.5469999999999999</v>
-      </c>
-      <c r="D33" s="49">
-        <f t="shared" si="1"/>
-        <v>6.6200000000000005E-4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="43" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="43" t="s">
-        <v>123</v>
-      </c>
-      <c r="B36" s="43" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="48" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A38" s="44" t="s">
-        <v>111</v>
-      </c>
-      <c r="B38" s="43" t="s">
-        <v>112</v>
-      </c>
-      <c r="C38" s="43" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A39" s="43" t="s">
-        <v>126</v>
-      </c>
-      <c r="B39" s="46">
-        <v>0.38600000000000001</v>
-      </c>
-      <c r="C39" s="42">
-        <v>-0.73099999999999998</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A40" s="43" t="s">
-        <v>126</v>
-      </c>
-      <c r="B40" s="46">
-        <v>0.38200000000000001</v>
-      </c>
-      <c r="C40" s="42">
-        <v>-0.72</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A41" s="43" t="s">
-        <v>126</v>
-      </c>
-      <c r="B41" s="46">
-        <v>0.38100000000000001</v>
-      </c>
-      <c r="C41" s="42">
-        <v>-0.71499999999999997</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A42" s="45">
-        <v>0</v>
-      </c>
-      <c r="B42" s="46">
-        <v>0.38200000000000001</v>
-      </c>
-      <c r="C42" s="45">
-        <v>0.72</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A43" s="45">
-        <v>1</v>
-      </c>
-      <c r="B43" s="46">
-        <v>0.39100000000000001</v>
-      </c>
-      <c r="C43" s="45">
-        <v>-0.751</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A44" s="45">
-        <v>2</v>
-      </c>
-      <c r="B44" s="46">
-        <v>0.4</v>
-      </c>
-      <c r="C44" s="45">
-        <v>-0.78300000000000003</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A45" s="45">
-        <v>3</v>
-      </c>
-      <c r="B45" s="46">
-        <v>0.41099999999999998</v>
-      </c>
-      <c r="C45" s="45">
-        <v>-0.81799999999999995</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A46" s="45">
-        <v>4</v>
-      </c>
-      <c r="B46" s="46">
-        <v>0.42099999999999999</v>
-      </c>
-      <c r="C46" s="45">
-        <v>-0.85499999999999998</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A47" s="45">
-        <v>5</v>
-      </c>
-      <c r="B47" s="46">
-        <v>0.436</v>
-      </c>
-      <c r="C47" s="45">
-        <v>-0.90100000000000002</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A48" s="45">
-        <v>6</v>
-      </c>
-      <c r="B48" s="46">
-        <v>0.498</v>
-      </c>
-      <c r="C48" s="45">
-        <v>-1.0680000000000001</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A49" s="45">
-        <v>7</v>
-      </c>
-      <c r="B49" s="46">
-        <v>0.57799999999999996</v>
-      </c>
-      <c r="C49" s="45">
-        <v>-1.226</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A50" s="45">
-        <v>7.5</v>
-      </c>
-      <c r="B50" s="46">
-        <v>0.61899999999999999</v>
-      </c>
-      <c r="C50" s="45">
-        <v>-1.3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="43" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="43" t="s">
-        <v>123</v>
-      </c>
-      <c r="B53" s="43" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="48" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A55" s="44" t="s">
-        <v>111</v>
-      </c>
-      <c r="B55" s="43" t="s">
-        <v>112</v>
-      </c>
-      <c r="C55" s="43" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A56" s="43" t="s">
-        <v>126</v>
-      </c>
-      <c r="B56" s="46">
-        <v>0.32700000000000001</v>
-      </c>
-      <c r="C56" s="42">
-        <v>-0.54</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A57" s="43" t="s">
-        <v>126</v>
-      </c>
-      <c r="B57" s="46">
-        <v>0.32300000000000001</v>
-      </c>
-      <c r="C57" s="42">
-        <v>-0.53400000000000003</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A58" s="43" t="s">
-        <v>126</v>
-      </c>
-      <c r="B58" s="46">
-        <v>0.32100000000000001</v>
-      </c>
-      <c r="C58" s="42">
-        <v>-0.53</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A59" s="45">
-        <v>0</v>
-      </c>
-      <c r="B59" s="46">
-        <v>0.315</v>
-      </c>
-      <c r="C59" s="45">
-        <v>-0.52800000000000002</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A60" s="45">
-        <v>1</v>
-      </c>
-      <c r="B60" s="46">
-        <v>0.34399999999999997</v>
-      </c>
-      <c r="C60" s="45">
-        <v>-0.59299999999999997</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A61" s="45">
-        <v>2</v>
-      </c>
-      <c r="B61" s="46">
-        <v>0.35799999999999998</v>
-      </c>
-      <c r="C61" s="45">
-        <v>-0.67400000000000004</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A62" s="45">
-        <v>3</v>
-      </c>
-      <c r="B62" s="46">
-        <v>0.38900000000000001</v>
-      </c>
-      <c r="C62" s="45">
-        <v>-0.76600000000000001</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A63" s="45">
-        <v>4</v>
-      </c>
-      <c r="B63" s="46">
-        <v>0.42599999999999999</v>
-      </c>
-      <c r="C63" s="45">
-        <v>-0.85599999999999998</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A64" s="45">
-        <v>5</v>
-      </c>
-      <c r="B64" s="46">
-        <v>0.46899999999999997</v>
-      </c>
-      <c r="C64" s="45">
-        <v>-0.94099999999999995</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A65" s="45">
-        <v>6</v>
-      </c>
-      <c r="B65" s="46">
-        <v>0.52400000000000002</v>
-      </c>
-      <c r="C65" s="45">
-        <v>-1.036</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A66" s="45">
-        <v>7</v>
-      </c>
-      <c r="B66" s="46">
-        <v>0.58899999999999997</v>
-      </c>
-      <c r="C66" s="45">
-        <v>-1.1479999999999999</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A67" s="45">
-        <v>7.5</v>
-      </c>
-      <c r="B67" s="46">
+      <c r="B119" s="38">
         <v>0.627</v>
       </c>
-      <c r="C67" s="45">
+      <c r="C119">
         <v>-1.212</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="B40:C40"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>